<commit_message>
Updated run for publication
</commit_message>
<xml_diff>
--- a/results/FrequencyTables/23974631_T5.xlsx
+++ b/results/FrequencyTables/23974631_T5.xlsx
@@ -465,73 +465,73 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.00226073850791258</v>
       </c>
       <c r="C2">
-        <v>0.0202020202020202</v>
+        <v>0.00301431801055011</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.014318010550113</v>
       </c>
       <c r="E2">
-        <v>0.98989898989899</v>
+        <v>0.957045968349661</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.0188394875659382</v>
       </c>
       <c r="G2">
-        <v>0.98989898989899</v>
+        <v>0.975131876412962</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.0158251695553881</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.012810851544838</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.969856819894499</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.00678221552373775</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0.972117558402411</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>0.00226073850791258</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>0.0105501130369254</v>
       </c>
       <c r="O2">
-        <v>0.0303030303030303</v>
+        <v>0.0504898266767144</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>0.00452147701582517</v>
       </c>
       <c r="Q2">
         <v>1</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>0.00602863602110023</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>0.000753579502637528</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>0.000753579502637528</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>0.00452147701582517</v>
       </c>
       <c r="V2">
-        <v>0.0101010101010101</v>
+        <v>0.0113036925395629</v>
       </c>
       <c r="W2">
-        <v>0.0101010101010101</v>
+        <v>0.00452147701582517</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>0.0173323285606631</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -539,46 +539,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.0188394875659382</v>
       </c>
       <c r="C3">
-        <v>0.0606060606060606</v>
+        <v>0.0278824415975885</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.0052750565184627</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.00226073850791258</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.00376789751318764</v>
       </c>
       <c r="H3">
-        <v>0.98989898989899</v>
+        <v>0.978146194423512</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0.970610399397136</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.0233609645817634</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>0.027128862094951</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.025621703089676</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>0.00226073850791258</v>
       </c>
       <c r="N3">
-        <v>0.676767676767677</v>
+        <v>0.859080633006782</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>0.0497362471740769</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -587,22 +587,22 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>0.0195930670685757</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>0.99698568198945</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>0.995478522984175</v>
       </c>
       <c r="U3">
-        <v>0.0404040404040404</v>
+        <v>0.0497362471740769</v>
       </c>
       <c r="V3">
         <v>0</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>0.0120572720422005</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -613,73 +613,73 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.970610399397136</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.00753579502637528</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.0120572720422005</v>
       </c>
       <c r="E4">
-        <v>0.0101010101010101</v>
+        <v>0.0293896006028636</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0.966842501883949</v>
       </c>
       <c r="G4">
-        <v>0.0101010101010101</v>
+        <v>0.0195930670685757</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.00301431801055011</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>0.00226073850791258</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0.961567445365486</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.00226073850791258</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>0.000753579502637528</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.00301431801055011</v>
       </c>
       <c r="O4">
-        <v>0.0101010101010101</v>
+        <v>0.00376789751318764</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0.995478522984175</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>0.972117558402411</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>0.000753579502637528</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>0.000753579502637528</v>
       </c>
       <c r="V4">
-        <v>0.98989898989899</v>
+        <v>0.974378296910324</v>
       </c>
       <c r="W4">
-        <v>0.98989898989899</v>
+        <v>0.970610399397136</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>0.968349660889224</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -687,46 +687,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.00753579502637528</v>
       </c>
       <c r="C5">
-        <v>0.919191919191919</v>
+        <v>0.961567445365486</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.968349660889224</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.0113036925395629</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.014318010550113</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.00150715900527506</v>
       </c>
       <c r="H5">
-        <v>0.0101010101010101</v>
+        <v>0.00602863602110023</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.0135644310474755</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.00452147701582517</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>0.00452147701582517</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0.994724943481537</v>
       </c>
       <c r="N5">
-        <v>0.323232323232323</v>
+        <v>0.127354935945742</v>
       </c>
       <c r="O5">
-        <v>0.95959595959596</v>
+        <v>0.896006028636021</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -735,25 +735,25 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>0.00150715900527506</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>0.00226073850791258</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>0.00301431801055011</v>
       </c>
       <c r="U5">
-        <v>0.95959595959596</v>
+        <v>0.94498869630746</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>0.0135644310474755</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>0.0120572720422005</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>0.014318010550113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>